<commit_message>
Hi Ramesh commiting with the logout action and fetching the URL
</commit_message>
<xml_diff>
--- a/TestData/MGFF_TestData.xlsx
+++ b/TestData/MGFF_TestData.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Logout" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Template" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="47">
   <si>
     <t xml:space="preserve">testNameDetails</t>
   </si>
@@ -147,10 +148,10 @@
     <t xml:space="preserve">Scholar</t>
   </si>
   <si>
-    <t xml:space="preserve">nd1432@BLR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shalini@Navadhiti.Com</t>
+    <t xml:space="preserve">validate login feature with login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate with logout</t>
   </si>
   <si>
     <t xml:space="preserve">templatename</t>
@@ -392,11 +393,11 @@
   </sheetPr>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="41.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="34.08"/>
@@ -619,56 +620,104 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="27.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="43.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="G2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="Shalini@Navadhiti.Com"/>
+    <hyperlink ref="E2" r:id="rId1" display="nd1432@blr"/>
+    <hyperlink ref="E3" r:id="rId2" display="nd1432@blr"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -687,11 +736,11 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P24" activeCellId="0" sqref="P24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.3"/>
@@ -774,4 +823,27 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>